<commit_message>
bug fix Privilige price removed from total report
</commit_message>
<xml_diff>
--- a/web/excel/period_report.xlsx
+++ b/web/excel/period_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\seating\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD59553E-0361-451C-A0DC-5ECBE31D6F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AD0191-DDC0-45FD-BFF2-E820B7E4655D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Сумма</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Наименование организации</t>
   </si>
   <si>
-    <t xml:space="preserve">Количество проданные билеты </t>
+    <t>Период:</t>
   </si>
   <si>
-    <t>Период:</t>
+    <t>Сумма проданных билетов</t>
+  </si>
+  <si>
+    <t>Сумма возвращенных билетов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">К-во проданные билеты </t>
+  </si>
+  <si>
+    <t>К-во возвращенные билеты</t>
   </si>
 </sst>
 </file>
@@ -437,249 +443,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.296875" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.19921875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="78.25" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9"/>
       <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="9"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
       <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="9"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9"/>
       <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9"/>
       <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9"/>
       <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="9"/>
       <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="9"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="9"/>
       <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="9"/>
       <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="9"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9"/>
       <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9"/>
       <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="9"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9"/>
       <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="9"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="9"/>
       <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="9"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="9"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="9"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="9"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="9"/>
       <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="9"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="9"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="9"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="9"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="9"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="9"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="9"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="9"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="9"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="9"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="9"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="9"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="9"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="9"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="9"/>
       <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="9"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="9"/>
       <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="9"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="9"/>
       <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="9"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="9"/>
       <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="9"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="9"/>
       <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="9"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="9"/>
       <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="9"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="9"/>
       <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="9"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="9"/>
       <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="9"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="9"/>
       <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="9"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="9"/>
       <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="9"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="9"/>
       <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="9"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="9"/>
       <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="9"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="9"/>
       <c r="C45" s="6"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>